<commit_message>
add pretty printed tables and fix some constraints
</commit_message>
<xml_diff>
--- a/assets/必开燃机列表.xlsx
+++ b/assets/必开燃机列表.xlsx
@@ -431,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:R161"/>
+  <dimension ref="A1:R148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,7 +495,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="1">
-        <v>44872.677083333336</v>
+        <v>44872.8125</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
@@ -517,7 +517,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="1">
-        <v>44872.6875</v>
+        <v>44872.822916666664</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -539,7 +539,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="1">
-        <v>44872.697916666664</v>
+        <v>44872.833333333336</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
@@ -561,7 +561,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="1">
-        <v>44872.708333333336</v>
+        <v>44872.84375</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
@@ -583,7 +583,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="1">
-        <v>44872.71875</v>
+        <v>44872.854166666664</v>
       </c>
       <c r="B6"/>
       <c r="C6"/>
@@ -605,7 +605,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="1">
-        <v>44872.729166666664</v>
+        <v>44872.864583333336</v>
       </c>
       <c r="B7"/>
       <c r="C7"/>
@@ -627,7 +627,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="1">
-        <v>44872.739583333336</v>
+        <v>44872.875</v>
       </c>
       <c r="B8"/>
       <c r="C8"/>
@@ -649,7 +649,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="1">
-        <v>44872.75</v>
+        <v>44872.885416666664</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -671,7 +671,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="1">
-        <v>44872.760416666664</v>
+        <v>44872.895833333336</v>
       </c>
       <c r="B10"/>
       <c r="C10"/>
@@ -693,7 +693,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="1">
-        <v>44872.770833333336</v>
+        <v>44872.90625</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
@@ -715,7 +715,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="1">
-        <v>44872.78125</v>
+        <v>44872.916666666664</v>
       </c>
       <c r="B12"/>
       <c r="C12"/>
@@ -737,7 +737,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="1">
-        <v>44872.791666666664</v>
+        <v>44872.927083333336</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
@@ -759,7 +759,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="1">
-        <v>44872.802083333336</v>
+        <v>44872.9375</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -781,7 +781,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="1">
-        <v>44872.8125</v>
+        <v>44872.947916666664</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -803,7 +803,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="1">
-        <v>44872.822916666664</v>
+        <v>44872.958333333336</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
@@ -825,7 +825,7 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="1">
-        <v>44872.833333333336</v>
+        <v>44872.96875</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -847,7 +847,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="1">
-        <v>44872.84375</v>
+        <v>44872.979166666664</v>
       </c>
       <c r="B18"/>
       <c r="C18"/>
@@ -869,7 +869,7 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="1">
-        <v>44872.854166666664</v>
+        <v>44872.989583333336</v>
       </c>
       <c r="B19"/>
       <c r="C19"/>
@@ -891,7 +891,7 @@
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="1">
-        <v>44872.864583333336</v>
+        <v>44873.0</v>
       </c>
       <c r="B20"/>
       <c r="C20"/>
@@ -913,7 +913,7 @@
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="1">
-        <v>44872.875</v>
+        <v>44873.010416666664</v>
       </c>
       <c r="B21"/>
       <c r="C21"/>
@@ -922,7 +922,9 @@
       <c r="F21"/>
       <c r="G21"/>
       <c r="H21"/>
-      <c r="I21"/>
+      <c r="I21">
+        <v>1</v>
+      </c>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
@@ -935,7 +937,7 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="1">
-        <v>44872.885416666664</v>
+        <v>44873.020833333336</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -944,7 +946,9 @@
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22"/>
-      <c r="I22"/>
+      <c r="I22">
+        <v>1</v>
+      </c>
       <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
@@ -957,7 +961,7 @@
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="1">
-        <v>44872.895833333336</v>
+        <v>44873.03125</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -966,7 +970,9 @@
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
-      <c r="I23"/>
+      <c r="I23">
+        <v>1</v>
+      </c>
       <c r="J23"/>
       <c r="K23"/>
       <c r="L23"/>
@@ -979,7 +985,7 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="1">
-        <v>44872.90625</v>
+        <v>44873.041666666664</v>
       </c>
       <c r="B24"/>
       <c r="C24"/>
@@ -988,7 +994,9 @@
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24"/>
-      <c r="I24"/>
+      <c r="I24">
+        <v>1</v>
+      </c>
       <c r="J24"/>
       <c r="K24"/>
       <c r="L24"/>
@@ -1001,7 +1009,7 @@
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="1">
-        <v>44872.916666666664</v>
+        <v>44873.052083333336</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -1010,7 +1018,9 @@
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25"/>
-      <c r="I25"/>
+      <c r="I25">
+        <v>1</v>
+      </c>
       <c r="J25"/>
       <c r="K25"/>
       <c r="L25"/>
@@ -1023,7 +1033,7 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="1">
-        <v>44872.927083333336</v>
+        <v>44873.0625</v>
       </c>
       <c r="B26"/>
       <c r="C26"/>
@@ -1032,7 +1042,9 @@
       <c r="F26"/>
       <c r="G26"/>
       <c r="H26"/>
-      <c r="I26"/>
+      <c r="I26">
+        <v>1</v>
+      </c>
       <c r="J26"/>
       <c r="K26"/>
       <c r="L26"/>
@@ -1045,7 +1057,7 @@
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="1">
-        <v>44872.9375</v>
+        <v>44873.072916666664</v>
       </c>
       <c r="B27"/>
       <c r="C27"/>
@@ -1054,7 +1066,9 @@
       <c r="F27"/>
       <c r="G27"/>
       <c r="H27"/>
-      <c r="I27"/>
+      <c r="I27">
+        <v>1</v>
+      </c>
       <c r="J27"/>
       <c r="K27"/>
       <c r="L27"/>
@@ -1067,7 +1081,7 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1">
-        <v>44872.947916666664</v>
+        <v>44873.083333333336</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
@@ -1076,7 +1090,9 @@
       <c r="F28"/>
       <c r="G28"/>
       <c r="H28"/>
-      <c r="I28"/>
+      <c r="I28">
+        <v>1</v>
+      </c>
       <c r="J28"/>
       <c r="K28"/>
       <c r="L28"/>
@@ -1089,7 +1105,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1">
-        <v>44872.958333333336</v>
+        <v>44873.09375</v>
       </c>
       <c r="B29"/>
       <c r="C29"/>
@@ -1098,7 +1114,9 @@
       <c r="F29"/>
       <c r="G29"/>
       <c r="H29"/>
-      <c r="I29"/>
+      <c r="I29">
+        <v>1</v>
+      </c>
       <c r="J29"/>
       <c r="K29"/>
       <c r="L29"/>
@@ -1111,7 +1129,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" s="1">
-        <v>44872.96875</v>
+        <v>44873.104166666664</v>
       </c>
       <c r="B30"/>
       <c r="C30"/>
@@ -1120,7 +1138,9 @@
       <c r="F30"/>
       <c r="G30"/>
       <c r="H30"/>
-      <c r="I30"/>
+      <c r="I30">
+        <v>1</v>
+      </c>
       <c r="J30"/>
       <c r="K30"/>
       <c r="L30"/>
@@ -1133,7 +1153,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" s="1">
-        <v>44872.979166666664</v>
+        <v>44873.114583333336</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -1142,7 +1162,9 @@
       <c r="F31"/>
       <c r="G31"/>
       <c r="H31"/>
-      <c r="I31"/>
+      <c r="I31">
+        <v>1</v>
+      </c>
       <c r="J31"/>
       <c r="K31"/>
       <c r="L31"/>
@@ -1155,7 +1177,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="1">
-        <v>44872.989583333336</v>
+        <v>44873.125</v>
       </c>
       <c r="B32"/>
       <c r="C32"/>
@@ -1164,7 +1186,9 @@
       <c r="F32"/>
       <c r="G32"/>
       <c r="H32"/>
-      <c r="I32"/>
+      <c r="I32">
+        <v>1</v>
+      </c>
       <c r="J32"/>
       <c r="K32"/>
       <c r="L32"/>
@@ -1177,7 +1201,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="1">
-        <v>44873.0</v>
+        <v>44873.135416666664</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
@@ -1186,7 +1210,9 @@
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33"/>
-      <c r="I33"/>
+      <c r="I33">
+        <v>1</v>
+      </c>
       <c r="J33"/>
       <c r="K33"/>
       <c r="L33"/>
@@ -1199,7 +1225,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" s="1">
-        <v>44873.010416666664</v>
+        <v>44873.145833333336</v>
       </c>
       <c r="B34"/>
       <c r="C34"/>
@@ -1223,7 +1249,7 @@
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="1">
-        <v>44873.020833333336</v>
+        <v>44873.15625</v>
       </c>
       <c r="B35"/>
       <c r="C35"/>
@@ -1247,7 +1273,7 @@
     </row>
     <row r="36" spans="1:18">
       <c r="A36" s="1">
-        <v>44873.03125</v>
+        <v>44873.166666666664</v>
       </c>
       <c r="B36"/>
       <c r="C36"/>
@@ -1271,7 +1297,7 @@
     </row>
     <row r="37" spans="1:18">
       <c r="A37" s="1">
-        <v>44873.041666666664</v>
+        <v>44873.177083333336</v>
       </c>
       <c r="B37"/>
       <c r="C37"/>
@@ -1295,7 +1321,7 @@
     </row>
     <row r="38" spans="1:18">
       <c r="A38" s="1">
-        <v>44873.052083333336</v>
+        <v>44873.1875</v>
       </c>
       <c r="B38"/>
       <c r="C38"/>
@@ -1319,7 +1345,7 @@
     </row>
     <row r="39" spans="1:18">
       <c r="A39" s="1">
-        <v>44873.0625</v>
+        <v>44873.197916666664</v>
       </c>
       <c r="B39"/>
       <c r="C39"/>
@@ -1343,7 +1369,7 @@
     </row>
     <row r="40" spans="1:18">
       <c r="A40" s="1">
-        <v>44873.072916666664</v>
+        <v>44873.208333333336</v>
       </c>
       <c r="B40"/>
       <c r="C40"/>
@@ -1367,7 +1393,7 @@
     </row>
     <row r="41" spans="1:18">
       <c r="A41" s="1">
-        <v>44873.083333333336</v>
+        <v>44873.21875</v>
       </c>
       <c r="B41"/>
       <c r="C41"/>
@@ -1391,7 +1417,7 @@
     </row>
     <row r="42" spans="1:18">
       <c r="A42" s="1">
-        <v>44873.09375</v>
+        <v>44873.229166666664</v>
       </c>
       <c r="B42"/>
       <c r="C42"/>
@@ -1415,7 +1441,7 @@
     </row>
     <row r="43" spans="1:18">
       <c r="A43" s="1">
-        <v>44873.104166666664</v>
+        <v>44873.239583333336</v>
       </c>
       <c r="B43"/>
       <c r="C43"/>
@@ -1439,7 +1465,7 @@
     </row>
     <row r="44" spans="1:18">
       <c r="A44" s="1">
-        <v>44873.114583333336</v>
+        <v>44873.25</v>
       </c>
       <c r="B44"/>
       <c r="C44"/>
@@ -1463,7 +1489,7 @@
     </row>
     <row r="45" spans="1:18">
       <c r="A45" s="1">
-        <v>44873.125</v>
+        <v>44873.260416666664</v>
       </c>
       <c r="B45"/>
       <c r="C45"/>
@@ -1487,7 +1513,7 @@
     </row>
     <row r="46" spans="1:18">
       <c r="A46" s="1">
-        <v>44873.135416666664</v>
+        <v>44873.270833333336</v>
       </c>
       <c r="B46"/>
       <c r="C46"/>
@@ -1511,7 +1537,7 @@
     </row>
     <row r="47" spans="1:18">
       <c r="A47" s="1">
-        <v>44873.145833333336</v>
+        <v>44873.28125</v>
       </c>
       <c r="B47"/>
       <c r="C47"/>
@@ -1535,7 +1561,7 @@
     </row>
     <row r="48" spans="1:18">
       <c r="A48" s="1">
-        <v>44873.15625</v>
+        <v>44873.291666666664</v>
       </c>
       <c r="B48"/>
       <c r="C48"/>
@@ -1559,7 +1585,7 @@
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="1">
-        <v>44873.166666666664</v>
+        <v>44873.302083333336</v>
       </c>
       <c r="B49"/>
       <c r="C49"/>
@@ -1583,7 +1609,7 @@
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="1">
-        <v>44873.177083333336</v>
+        <v>44873.3125</v>
       </c>
       <c r="B50"/>
       <c r="C50"/>
@@ -1607,7 +1633,7 @@
     </row>
     <row r="51" spans="1:18">
       <c r="A51" s="1">
-        <v>44873.1875</v>
+        <v>44873.322916666664</v>
       </c>
       <c r="B51"/>
       <c r="C51"/>
@@ -1631,7 +1657,7 @@
     </row>
     <row r="52" spans="1:18">
       <c r="A52" s="1">
-        <v>44873.197916666664</v>
+        <v>44873.333333333336</v>
       </c>
       <c r="B52"/>
       <c r="C52"/>
@@ -1655,7 +1681,7 @@
     </row>
     <row r="53" spans="1:18">
       <c r="A53" s="1">
-        <v>44873.208333333336</v>
+        <v>44873.34375</v>
       </c>
       <c r="B53"/>
       <c r="C53"/>
@@ -1664,9 +1690,7 @@
       <c r="F53"/>
       <c r="G53"/>
       <c r="H53"/>
-      <c r="I53">
-        <v>1</v>
-      </c>
+      <c r="I53"/>
       <c r="J53"/>
       <c r="K53"/>
       <c r="L53"/>
@@ -1679,7 +1703,7 @@
     </row>
     <row r="54" spans="1:18">
       <c r="A54" s="1">
-        <v>44873.21875</v>
+        <v>44873.354166666664</v>
       </c>
       <c r="B54"/>
       <c r="C54"/>
@@ -1688,9 +1712,7 @@
       <c r="F54"/>
       <c r="G54"/>
       <c r="H54"/>
-      <c r="I54">
-        <v>1</v>
-      </c>
+      <c r="I54"/>
       <c r="J54"/>
       <c r="K54"/>
       <c r="L54"/>
@@ -1703,7 +1725,7 @@
     </row>
     <row r="55" spans="1:18">
       <c r="A55" s="1">
-        <v>44873.229166666664</v>
+        <v>44873.364583333336</v>
       </c>
       <c r="B55"/>
       <c r="C55"/>
@@ -1712,9 +1734,7 @@
       <c r="F55"/>
       <c r="G55"/>
       <c r="H55"/>
-      <c r="I55">
-        <v>1</v>
-      </c>
+      <c r="I55"/>
       <c r="J55"/>
       <c r="K55"/>
       <c r="L55"/>
@@ -1727,7 +1747,7 @@
     </row>
     <row r="56" spans="1:18">
       <c r="A56" s="1">
-        <v>44873.239583333336</v>
+        <v>44873.375</v>
       </c>
       <c r="B56"/>
       <c r="C56"/>
@@ -1736,9 +1756,7 @@
       <c r="F56"/>
       <c r="G56"/>
       <c r="H56"/>
-      <c r="I56">
-        <v>1</v>
-      </c>
+      <c r="I56"/>
       <c r="J56"/>
       <c r="K56"/>
       <c r="L56"/>
@@ -1751,7 +1769,7 @@
     </row>
     <row r="57" spans="1:18">
       <c r="A57" s="1">
-        <v>44873.25</v>
+        <v>44873.385416666664</v>
       </c>
       <c r="B57"/>
       <c r="C57"/>
@@ -1760,9 +1778,7 @@
       <c r="F57"/>
       <c r="G57"/>
       <c r="H57"/>
-      <c r="I57">
-        <v>1</v>
-      </c>
+      <c r="I57"/>
       <c r="J57"/>
       <c r="K57"/>
       <c r="L57"/>
@@ -1775,7 +1791,7 @@
     </row>
     <row r="58" spans="1:18">
       <c r="A58" s="1">
-        <v>44873.260416666664</v>
+        <v>44873.395833333336</v>
       </c>
       <c r="B58"/>
       <c r="C58"/>
@@ -1784,9 +1800,7 @@
       <c r="F58"/>
       <c r="G58"/>
       <c r="H58"/>
-      <c r="I58">
-        <v>1</v>
-      </c>
+      <c r="I58"/>
       <c r="J58"/>
       <c r="K58"/>
       <c r="L58"/>
@@ -1799,7 +1813,7 @@
     </row>
     <row r="59" spans="1:18">
       <c r="A59" s="1">
-        <v>44873.270833333336</v>
+        <v>44873.40625</v>
       </c>
       <c r="B59"/>
       <c r="C59"/>
@@ -1808,9 +1822,7 @@
       <c r="F59"/>
       <c r="G59"/>
       <c r="H59"/>
-      <c r="I59">
-        <v>1</v>
-      </c>
+      <c r="I59"/>
       <c r="J59"/>
       <c r="K59"/>
       <c r="L59"/>
@@ -1823,7 +1835,7 @@
     </row>
     <row r="60" spans="1:18">
       <c r="A60" s="1">
-        <v>44873.28125</v>
+        <v>44873.416666666664</v>
       </c>
       <c r="B60"/>
       <c r="C60"/>
@@ -1832,9 +1844,7 @@
       <c r="F60"/>
       <c r="G60"/>
       <c r="H60"/>
-      <c r="I60">
-        <v>1</v>
-      </c>
+      <c r="I60"/>
       <c r="J60"/>
       <c r="K60"/>
       <c r="L60"/>
@@ -1847,7 +1857,7 @@
     </row>
     <row r="61" spans="1:18">
       <c r="A61" s="1">
-        <v>44873.291666666664</v>
+        <v>44873.427083333336</v>
       </c>
       <c r="B61"/>
       <c r="C61"/>
@@ -1856,9 +1866,7 @@
       <c r="F61"/>
       <c r="G61"/>
       <c r="H61"/>
-      <c r="I61">
-        <v>1</v>
-      </c>
+      <c r="I61"/>
       <c r="J61"/>
       <c r="K61"/>
       <c r="L61"/>
@@ -1871,7 +1879,7 @@
     </row>
     <row r="62" spans="1:18">
       <c r="A62" s="1">
-        <v>44873.302083333336</v>
+        <v>44873.4375</v>
       </c>
       <c r="B62"/>
       <c r="C62"/>
@@ -1880,9 +1888,7 @@
       <c r="F62"/>
       <c r="G62"/>
       <c r="H62"/>
-      <c r="I62">
-        <v>1</v>
-      </c>
+      <c r="I62"/>
       <c r="J62"/>
       <c r="K62"/>
       <c r="L62"/>
@@ -1895,7 +1901,7 @@
     </row>
     <row r="63" spans="1:18">
       <c r="A63" s="1">
-        <v>44873.3125</v>
+        <v>44873.447916666664</v>
       </c>
       <c r="B63"/>
       <c r="C63"/>
@@ -1904,9 +1910,7 @@
       <c r="F63"/>
       <c r="G63"/>
       <c r="H63"/>
-      <c r="I63">
-        <v>1</v>
-      </c>
+      <c r="I63"/>
       <c r="J63"/>
       <c r="K63"/>
       <c r="L63"/>
@@ -1919,7 +1923,7 @@
     </row>
     <row r="64" spans="1:18">
       <c r="A64" s="1">
-        <v>44873.322916666664</v>
+        <v>44873.458333333336</v>
       </c>
       <c r="B64"/>
       <c r="C64"/>
@@ -1928,9 +1932,7 @@
       <c r="F64"/>
       <c r="G64"/>
       <c r="H64"/>
-      <c r="I64">
-        <v>1</v>
-      </c>
+      <c r="I64"/>
       <c r="J64"/>
       <c r="K64"/>
       <c r="L64"/>
@@ -1943,7 +1945,7 @@
     </row>
     <row r="65" spans="1:18">
       <c r="A65" s="1">
-        <v>44873.333333333336</v>
+        <v>44873.46875</v>
       </c>
       <c r="B65"/>
       <c r="C65"/>
@@ -1952,9 +1954,7 @@
       <c r="F65"/>
       <c r="G65"/>
       <c r="H65"/>
-      <c r="I65">
-        <v>1</v>
-      </c>
+      <c r="I65"/>
       <c r="J65"/>
       <c r="K65"/>
       <c r="L65"/>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="66" spans="1:18">
       <c r="A66" s="1">
-        <v>44873.34375</v>
+        <v>44873.479166666664</v>
       </c>
       <c r="B66"/>
       <c r="C66"/>
@@ -1989,7 +1989,7 @@
     </row>
     <row r="67" spans="1:18">
       <c r="A67" s="1">
-        <v>44873.354166666664</v>
+        <v>44873.489583333336</v>
       </c>
       <c r="B67"/>
       <c r="C67"/>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="68" spans="1:18">
       <c r="A68" s="1">
-        <v>44873.364583333336</v>
+        <v>44873.5</v>
       </c>
       <c r="B68"/>
       <c r="C68"/>
@@ -2033,7 +2033,7 @@
     </row>
     <row r="69" spans="1:18">
       <c r="A69" s="1">
-        <v>44873.375</v>
+        <v>44873.510416666664</v>
       </c>
       <c r="B69"/>
       <c r="C69"/>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="70" spans="1:18">
       <c r="A70" s="1">
-        <v>44873.385416666664</v>
+        <v>44873.520833333336</v>
       </c>
       <c r="B70"/>
       <c r="C70"/>
@@ -2077,7 +2077,7 @@
     </row>
     <row r="71" spans="1:18">
       <c r="A71" s="1">
-        <v>44873.395833333336</v>
+        <v>44873.53125</v>
       </c>
       <c r="B71"/>
       <c r="C71"/>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="72" spans="1:18">
       <c r="A72" s="1">
-        <v>44873.40625</v>
+        <v>44873.541666666664</v>
       </c>
       <c r="B72"/>
       <c r="C72"/>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="73" spans="1:18">
       <c r="A73" s="1">
-        <v>44873.416666666664</v>
+        <v>44873.552083333336</v>
       </c>
       <c r="B73"/>
       <c r="C73"/>
@@ -2143,7 +2143,7 @@
     </row>
     <row r="74" spans="1:18">
       <c r="A74" s="1">
-        <v>44873.427083333336</v>
+        <v>44873.5625</v>
       </c>
       <c r="B74"/>
       <c r="C74"/>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="75" spans="1:18">
       <c r="A75" s="1">
-        <v>44873.4375</v>
+        <v>44873.572916666664</v>
       </c>
       <c r="B75"/>
       <c r="C75"/>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="76" spans="1:18">
       <c r="A76" s="1">
-        <v>44873.447916666664</v>
+        <v>44873.583333333336</v>
       </c>
       <c r="B76"/>
       <c r="C76"/>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="77" spans="1:18">
       <c r="A77" s="1">
-        <v>44873.458333333336</v>
+        <v>44873.59375</v>
       </c>
       <c r="B77"/>
       <c r="C77"/>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="78" spans="1:18">
       <c r="A78" s="1">
-        <v>44873.46875</v>
+        <v>44873.604166666664</v>
       </c>
       <c r="B78"/>
       <c r="C78"/>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="79" spans="1:18">
       <c r="A79" s="1">
-        <v>44873.479166666664</v>
+        <v>44873.614583333336</v>
       </c>
       <c r="B79"/>
       <c r="C79"/>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="80" spans="1:18">
       <c r="A80" s="1">
-        <v>44873.489583333336</v>
+        <v>44873.625</v>
       </c>
       <c r="B80"/>
       <c r="C80"/>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="81" spans="1:18">
       <c r="A81" s="1">
-        <v>44873.5</v>
+        <v>44873.635416666664</v>
       </c>
       <c r="B81"/>
       <c r="C81"/>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="82" spans="1:18">
       <c r="A82" s="1">
-        <v>44873.510416666664</v>
+        <v>44873.645833333336</v>
       </c>
       <c r="B82"/>
       <c r="C82"/>
@@ -2341,7 +2341,7 @@
     </row>
     <row r="83" spans="1:18">
       <c r="A83" s="1">
-        <v>44873.520833333336</v>
+        <v>44873.65625</v>
       </c>
       <c r="B83"/>
       <c r="C83"/>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="84" spans="1:18">
       <c r="A84" s="1">
-        <v>44873.53125</v>
+        <v>44873.666666666664</v>
       </c>
       <c r="B84"/>
       <c r="C84"/>
@@ -2385,7 +2385,7 @@
     </row>
     <row r="85" spans="1:18">
       <c r="A85" s="1">
-        <v>44873.541666666664</v>
+        <v>44873.677083333336</v>
       </c>
       <c r="B85"/>
       <c r="C85"/>
@@ -2407,7 +2407,7 @@
     </row>
     <row r="86" spans="1:18">
       <c r="A86" s="1">
-        <v>44873.552083333336</v>
+        <v>44873.6875</v>
       </c>
       <c r="B86"/>
       <c r="C86"/>
@@ -2429,7 +2429,7 @@
     </row>
     <row r="87" spans="1:18">
       <c r="A87" s="1">
-        <v>44873.5625</v>
+        <v>44873.697916666664</v>
       </c>
       <c r="B87"/>
       <c r="C87"/>
@@ -2451,7 +2451,7 @@
     </row>
     <row r="88" spans="1:18">
       <c r="A88" s="1">
-        <v>44873.572916666664</v>
+        <v>44873.708333333336</v>
       </c>
       <c r="B88"/>
       <c r="C88"/>
@@ -2473,7 +2473,7 @@
     </row>
     <row r="89" spans="1:18">
       <c r="A89" s="1">
-        <v>44873.583333333336</v>
+        <v>44873.71875</v>
       </c>
       <c r="B89"/>
       <c r="C89"/>
@@ -2495,7 +2495,7 @@
     </row>
     <row r="90" spans="1:18">
       <c r="A90" s="1">
-        <v>44873.59375</v>
+        <v>44873.729166666664</v>
       </c>
       <c r="B90"/>
       <c r="C90"/>
@@ -2517,7 +2517,7 @@
     </row>
     <row r="91" spans="1:18">
       <c r="A91" s="1">
-        <v>44873.604166666664</v>
+        <v>44873.739583333336</v>
       </c>
       <c r="B91"/>
       <c r="C91"/>
@@ -2539,7 +2539,7 @@
     </row>
     <row r="92" spans="1:18">
       <c r="A92" s="1">
-        <v>44873.614583333336</v>
+        <v>44873.75</v>
       </c>
       <c r="B92"/>
       <c r="C92"/>
@@ -2561,7 +2561,7 @@
     </row>
     <row r="93" spans="1:18">
       <c r="A93" s="1">
-        <v>44873.625</v>
+        <v>44873.760416666664</v>
       </c>
       <c r="B93"/>
       <c r="C93"/>
@@ -2583,7 +2583,7 @@
     </row>
     <row r="94" spans="1:18">
       <c r="A94" s="1">
-        <v>44873.635416666664</v>
+        <v>44873.770833333336</v>
       </c>
       <c r="B94"/>
       <c r="C94"/>
@@ -2605,7 +2605,7 @@
     </row>
     <row r="95" spans="1:18">
       <c r="A95" s="1">
-        <v>44873.645833333336</v>
+        <v>44873.78125</v>
       </c>
       <c r="B95"/>
       <c r="C95"/>
@@ -2627,7 +2627,7 @@
     </row>
     <row r="96" spans="1:18">
       <c r="A96" s="1">
-        <v>44873.65625</v>
+        <v>44873.791666666664</v>
       </c>
       <c r="B96"/>
       <c r="C96"/>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="97" spans="1:18">
       <c r="A97" s="1">
-        <v>44873.666666666664</v>
+        <v>44873.802083333336</v>
       </c>
       <c r="B97"/>
       <c r="C97"/>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="98" spans="1:18">
       <c r="A98" s="1">
-        <v>44873.677083333336</v>
+        <v>44873.8125</v>
       </c>
       <c r="B98"/>
       <c r="C98"/>
@@ -2693,7 +2693,7 @@
     </row>
     <row r="99" spans="1:18">
       <c r="A99" s="1">
-        <v>44873.6875</v>
+        <v>44873.822916666664</v>
       </c>
       <c r="B99"/>
       <c r="C99"/>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="100" spans="1:18">
       <c r="A100" s="1">
-        <v>44873.697916666664</v>
+        <v>44873.833333333336</v>
       </c>
       <c r="B100"/>
       <c r="C100"/>
@@ -2737,7 +2737,7 @@
     </row>
     <row r="101" spans="1:18">
       <c r="A101" s="1">
-        <v>44873.708333333336</v>
+        <v>44873.84375</v>
       </c>
       <c r="B101"/>
       <c r="C101"/>
@@ -2759,7 +2759,7 @@
     </row>
     <row r="102" spans="1:18">
       <c r="A102" s="1">
-        <v>44873.71875</v>
+        <v>44873.854166666664</v>
       </c>
       <c r="B102"/>
       <c r="C102"/>
@@ -2781,7 +2781,7 @@
     </row>
     <row r="103" spans="1:18">
       <c r="A103" s="1">
-        <v>44873.729166666664</v>
+        <v>44873.864583333336</v>
       </c>
       <c r="B103"/>
       <c r="C103"/>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="104" spans="1:18">
       <c r="A104" s="1">
-        <v>44873.739583333336</v>
+        <v>44873.875</v>
       </c>
       <c r="B104"/>
       <c r="C104"/>
@@ -2825,7 +2825,7 @@
     </row>
     <row r="105" spans="1:18">
       <c r="A105" s="1">
-        <v>44873.75</v>
+        <v>44873.885416666664</v>
       </c>
       <c r="B105"/>
       <c r="C105"/>
@@ -2847,7 +2847,7 @@
     </row>
     <row r="106" spans="1:18">
       <c r="A106" s="1">
-        <v>44873.760416666664</v>
+        <v>44873.895833333336</v>
       </c>
       <c r="B106"/>
       <c r="C106"/>
@@ -2869,7 +2869,7 @@
     </row>
     <row r="107" spans="1:18">
       <c r="A107" s="1">
-        <v>44873.770833333336</v>
+        <v>44873.90625</v>
       </c>
       <c r="B107"/>
       <c r="C107"/>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="108" spans="1:18">
       <c r="A108" s="1">
-        <v>44873.78125</v>
+        <v>44873.916666666664</v>
       </c>
       <c r="B108"/>
       <c r="C108"/>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="109" spans="1:18">
       <c r="A109" s="1">
-        <v>44873.791666666664</v>
+        <v>44873.927083333336</v>
       </c>
       <c r="B109"/>
       <c r="C109"/>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="110" spans="1:18">
       <c r="A110" s="1">
-        <v>44873.802083333336</v>
+        <v>44873.9375</v>
       </c>
       <c r="B110"/>
       <c r="C110"/>
@@ -2957,7 +2957,7 @@
     </row>
     <row r="111" spans="1:18">
       <c r="A111" s="1">
-        <v>44873.8125</v>
+        <v>44873.947916666664</v>
       </c>
       <c r="B111"/>
       <c r="C111"/>
@@ -2979,7 +2979,7 @@
     </row>
     <row r="112" spans="1:18">
       <c r="A112" s="1">
-        <v>44873.822916666664</v>
+        <v>44873.958333333336</v>
       </c>
       <c r="B112"/>
       <c r="C112"/>
@@ -3001,7 +3001,7 @@
     </row>
     <row r="113" spans="1:18">
       <c r="A113" s="1">
-        <v>44873.833333333336</v>
+        <v>44873.96875</v>
       </c>
       <c r="B113"/>
       <c r="C113"/>
@@ -3023,7 +3023,7 @@
     </row>
     <row r="114" spans="1:18">
       <c r="A114" s="1">
-        <v>44873.84375</v>
+        <v>44873.979166666664</v>
       </c>
       <c r="B114"/>
       <c r="C114"/>
@@ -3045,7 +3045,7 @@
     </row>
     <row r="115" spans="1:18">
       <c r="A115" s="1">
-        <v>44873.854166666664</v>
+        <v>44873.989583333336</v>
       </c>
       <c r="B115"/>
       <c r="C115"/>
@@ -3067,7 +3067,7 @@
     </row>
     <row r="116" spans="1:18">
       <c r="A116" s="1">
-        <v>44873.864583333336</v>
+        <v>44874.0</v>
       </c>
       <c r="B116"/>
       <c r="C116"/>
@@ -3089,7 +3089,7 @@
     </row>
     <row r="117" spans="1:18">
       <c r="A117" s="1">
-        <v>44873.875</v>
+        <v>44874.010416666664</v>
       </c>
       <c r="B117"/>
       <c r="C117"/>
@@ -3111,7 +3111,7 @@
     </row>
     <row r="118" spans="1:18">
       <c r="A118" s="1">
-        <v>44873.885416666664</v>
+        <v>44874.020833333336</v>
       </c>
       <c r="B118"/>
       <c r="C118"/>
@@ -3133,7 +3133,7 @@
     </row>
     <row r="119" spans="1:18">
       <c r="A119" s="1">
-        <v>44873.895833333336</v>
+        <v>44874.03125</v>
       </c>
       <c r="B119"/>
       <c r="C119"/>
@@ -3155,7 +3155,7 @@
     </row>
     <row r="120" spans="1:18">
       <c r="A120" s="1">
-        <v>44873.90625</v>
+        <v>44874.041666666664</v>
       </c>
       <c r="B120"/>
       <c r="C120"/>
@@ -3177,7 +3177,7 @@
     </row>
     <row r="121" spans="1:18">
       <c r="A121" s="1">
-        <v>44873.916666666664</v>
+        <v>44874.052083333336</v>
       </c>
       <c r="B121"/>
       <c r="C121"/>
@@ -3199,7 +3199,7 @@
     </row>
     <row r="122" spans="1:18">
       <c r="A122" s="1">
-        <v>44873.927083333336</v>
+        <v>44874.0625</v>
       </c>
       <c r="B122"/>
       <c r="C122"/>
@@ -3221,7 +3221,7 @@
     </row>
     <row r="123" spans="1:18">
       <c r="A123" s="1">
-        <v>44873.9375</v>
+        <v>44874.072916666664</v>
       </c>
       <c r="B123"/>
       <c r="C123"/>
@@ -3243,7 +3243,7 @@
     </row>
     <row r="124" spans="1:18">
       <c r="A124" s="1">
-        <v>44873.947916666664</v>
+        <v>44874.083333333336</v>
       </c>
       <c r="B124"/>
       <c r="C124"/>
@@ -3265,7 +3265,7 @@
     </row>
     <row r="125" spans="1:18">
       <c r="A125" s="1">
-        <v>44873.958333333336</v>
+        <v>44874.09375</v>
       </c>
       <c r="B125"/>
       <c r="C125"/>
@@ -3287,7 +3287,7 @@
     </row>
     <row r="126" spans="1:18">
       <c r="A126" s="1">
-        <v>44873.96875</v>
+        <v>44874.104166666664</v>
       </c>
       <c r="B126"/>
       <c r="C126"/>
@@ -3309,7 +3309,7 @@
     </row>
     <row r="127" spans="1:18">
       <c r="A127" s="1">
-        <v>44873.979166666664</v>
+        <v>44874.114583333336</v>
       </c>
       <c r="B127"/>
       <c r="C127"/>
@@ -3331,7 +3331,7 @@
     </row>
     <row r="128" spans="1:18">
       <c r="A128" s="1">
-        <v>44873.989583333336</v>
+        <v>44874.125</v>
       </c>
       <c r="B128"/>
       <c r="C128"/>
@@ -3353,7 +3353,7 @@
     </row>
     <row r="129" spans="1:18">
       <c r="A129" s="1">
-        <v>44874.0</v>
+        <v>44874.135416666664</v>
       </c>
       <c r="B129"/>
       <c r="C129"/>
@@ -3375,7 +3375,7 @@
     </row>
     <row r="130" spans="1:18">
       <c r="A130" s="1">
-        <v>44874.010416666664</v>
+        <v>44874.145833333336</v>
       </c>
       <c r="B130"/>
       <c r="C130"/>
@@ -3397,7 +3397,7 @@
     </row>
     <row r="131" spans="1:18">
       <c r="A131" s="1">
-        <v>44874.020833333336</v>
+        <v>44874.15625</v>
       </c>
       <c r="B131"/>
       <c r="C131"/>
@@ -3419,7 +3419,7 @@
     </row>
     <row r="132" spans="1:18">
       <c r="A132" s="1">
-        <v>44874.03125</v>
+        <v>44874.166666666664</v>
       </c>
       <c r="B132"/>
       <c r="C132"/>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="133" spans="1:18">
       <c r="A133" s="1">
-        <v>44874.041666666664</v>
+        <v>44874.177083333336</v>
       </c>
       <c r="B133"/>
       <c r="C133"/>
@@ -3463,7 +3463,7 @@
     </row>
     <row r="134" spans="1:18">
       <c r="A134" s="1">
-        <v>44874.052083333336</v>
+        <v>44874.1875</v>
       </c>
       <c r="B134"/>
       <c r="C134"/>
@@ -3485,7 +3485,7 @@
     </row>
     <row r="135" spans="1:18">
       <c r="A135" s="1">
-        <v>44874.0625</v>
+        <v>44874.197916666664</v>
       </c>
       <c r="B135"/>
       <c r="C135"/>
@@ -3507,7 +3507,7 @@
     </row>
     <row r="136" spans="1:18">
       <c r="A136" s="1">
-        <v>44874.072916666664</v>
+        <v>44874.208333333336</v>
       </c>
       <c r="B136"/>
       <c r="C136"/>
@@ -3529,7 +3529,7 @@
     </row>
     <row r="137" spans="1:18">
       <c r="A137" s="1">
-        <v>44874.083333333336</v>
+        <v>44874.21875</v>
       </c>
       <c r="B137"/>
       <c r="C137"/>
@@ -3551,7 +3551,7 @@
     </row>
     <row r="138" spans="1:18">
       <c r="A138" s="1">
-        <v>44874.09375</v>
+        <v>44874.229166666664</v>
       </c>
       <c r="B138"/>
       <c r="C138"/>
@@ -3573,7 +3573,7 @@
     </row>
     <row r="139" spans="1:18">
       <c r="A139" s="1">
-        <v>44874.104166666664</v>
+        <v>44874.239583333336</v>
       </c>
       <c r="B139"/>
       <c r="C139"/>
@@ -3595,7 +3595,7 @@
     </row>
     <row r="140" spans="1:18">
       <c r="A140" s="1">
-        <v>44874.114583333336</v>
+        <v>44874.25</v>
       </c>
       <c r="B140"/>
       <c r="C140"/>
@@ -3617,7 +3617,7 @@
     </row>
     <row r="141" spans="1:18">
       <c r="A141" s="1">
-        <v>44874.125</v>
+        <v>44874.260416666664</v>
       </c>
       <c r="B141"/>
       <c r="C141"/>
@@ -3639,7 +3639,7 @@
     </row>
     <row r="142" spans="1:18">
       <c r="A142" s="1">
-        <v>44874.135416666664</v>
+        <v>44874.270833333336</v>
       </c>
       <c r="B142"/>
       <c r="C142"/>
@@ -3661,7 +3661,7 @@
     </row>
     <row r="143" spans="1:18">
       <c r="A143" s="1">
-        <v>44874.145833333336</v>
+        <v>44874.28125</v>
       </c>
       <c r="B143"/>
       <c r="C143"/>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="144" spans="1:18">
       <c r="A144" s="1">
-        <v>44874.15625</v>
+        <v>44874.291666666664</v>
       </c>
       <c r="B144"/>
       <c r="C144"/>
@@ -3705,7 +3705,7 @@
     </row>
     <row r="145" spans="1:18">
       <c r="A145" s="1">
-        <v>44874.166666666664</v>
+        <v>44874.302083333336</v>
       </c>
       <c r="B145"/>
       <c r="C145"/>
@@ -3727,7 +3727,7 @@
     </row>
     <row r="146" spans="1:18">
       <c r="A146" s="1">
-        <v>44874.177083333336</v>
+        <v>44874.3125</v>
       </c>
       <c r="B146"/>
       <c r="C146"/>
@@ -3749,7 +3749,7 @@
     </row>
     <row r="147" spans="1:18">
       <c r="A147" s="1">
-        <v>44874.1875</v>
+        <v>44874.322916666664</v>
       </c>
       <c r="B147"/>
       <c r="C147"/>
@@ -3771,7 +3771,7 @@
     </row>
     <row r="148" spans="1:18">
       <c r="A148" s="1">
-        <v>44874.197916666664</v>
+        <v>44874.333333333336</v>
       </c>
       <c r="B148"/>
       <c r="C148"/>
@@ -3791,292 +3791,6 @@
       <c r="Q148"/>
       <c r="R148"/>
     </row>
-    <row r="149" spans="1:18">
-      <c r="A149" s="1">
-        <v>44874.208333333336</v>
-      </c>
-      <c r="B149"/>
-      <c r="C149"/>
-      <c r="D149"/>
-      <c r="E149"/>
-      <c r="F149"/>
-      <c r="G149"/>
-      <c r="H149"/>
-      <c r="I149"/>
-      <c r="J149"/>
-      <c r="K149"/>
-      <c r="L149"/>
-      <c r="M149"/>
-      <c r="N149"/>
-      <c r="O149"/>
-      <c r="P149"/>
-      <c r="Q149"/>
-      <c r="R149"/>
-    </row>
-    <row r="150" spans="1:18">
-      <c r="A150" s="1">
-        <v>44874.21875</v>
-      </c>
-      <c r="B150"/>
-      <c r="C150"/>
-      <c r="D150"/>
-      <c r="E150"/>
-      <c r="F150"/>
-      <c r="G150"/>
-      <c r="H150"/>
-      <c r="I150"/>
-      <c r="J150"/>
-      <c r="K150"/>
-      <c r="L150"/>
-      <c r="M150"/>
-      <c r="N150"/>
-      <c r="O150"/>
-      <c r="P150"/>
-      <c r="Q150"/>
-      <c r="R150"/>
-    </row>
-    <row r="151" spans="1:18">
-      <c r="A151" s="1">
-        <v>44874.229166666664</v>
-      </c>
-      <c r="B151"/>
-      <c r="C151"/>
-      <c r="D151"/>
-      <c r="E151"/>
-      <c r="F151"/>
-      <c r="G151"/>
-      <c r="H151"/>
-      <c r="I151"/>
-      <c r="J151"/>
-      <c r="K151"/>
-      <c r="L151"/>
-      <c r="M151"/>
-      <c r="N151"/>
-      <c r="O151"/>
-      <c r="P151"/>
-      <c r="Q151"/>
-      <c r="R151"/>
-    </row>
-    <row r="152" spans="1:18">
-      <c r="A152" s="1">
-        <v>44874.239583333336</v>
-      </c>
-      <c r="B152"/>
-      <c r="C152"/>
-      <c r="D152"/>
-      <c r="E152"/>
-      <c r="F152"/>
-      <c r="G152"/>
-      <c r="H152"/>
-      <c r="I152"/>
-      <c r="J152"/>
-      <c r="K152"/>
-      <c r="L152"/>
-      <c r="M152"/>
-      <c r="N152"/>
-      <c r="O152"/>
-      <c r="P152"/>
-      <c r="Q152"/>
-      <c r="R152"/>
-    </row>
-    <row r="153" spans="1:18">
-      <c r="A153" s="1">
-        <v>44874.25</v>
-      </c>
-      <c r="B153"/>
-      <c r="C153"/>
-      <c r="D153"/>
-      <c r="E153"/>
-      <c r="F153"/>
-      <c r="G153"/>
-      <c r="H153"/>
-      <c r="I153"/>
-      <c r="J153"/>
-      <c r="K153"/>
-      <c r="L153"/>
-      <c r="M153"/>
-      <c r="N153"/>
-      <c r="O153"/>
-      <c r="P153"/>
-      <c r="Q153"/>
-      <c r="R153"/>
-    </row>
-    <row r="154" spans="1:18">
-      <c r="A154" s="1">
-        <v>44874.260416666664</v>
-      </c>
-      <c r="B154"/>
-      <c r="C154"/>
-      <c r="D154"/>
-      <c r="E154"/>
-      <c r="F154"/>
-      <c r="G154"/>
-      <c r="H154"/>
-      <c r="I154"/>
-      <c r="J154"/>
-      <c r="K154"/>
-      <c r="L154"/>
-      <c r="M154"/>
-      <c r="N154"/>
-      <c r="O154"/>
-      <c r="P154"/>
-      <c r="Q154"/>
-      <c r="R154"/>
-    </row>
-    <row r="155" spans="1:18">
-      <c r="A155" s="1">
-        <v>44874.270833333336</v>
-      </c>
-      <c r="B155"/>
-      <c r="C155"/>
-      <c r="D155"/>
-      <c r="E155"/>
-      <c r="F155"/>
-      <c r="G155"/>
-      <c r="H155"/>
-      <c r="I155"/>
-      <c r="J155"/>
-      <c r="K155"/>
-      <c r="L155"/>
-      <c r="M155"/>
-      <c r="N155"/>
-      <c r="O155"/>
-      <c r="P155"/>
-      <c r="Q155"/>
-      <c r="R155"/>
-    </row>
-    <row r="156" spans="1:18">
-      <c r="A156" s="1">
-        <v>44874.28125</v>
-      </c>
-      <c r="B156"/>
-      <c r="C156"/>
-      <c r="D156"/>
-      <c r="E156"/>
-      <c r="F156"/>
-      <c r="G156"/>
-      <c r="H156"/>
-      <c r="I156"/>
-      <c r="J156"/>
-      <c r="K156"/>
-      <c r="L156"/>
-      <c r="M156"/>
-      <c r="N156"/>
-      <c r="O156"/>
-      <c r="P156"/>
-      <c r="Q156"/>
-      <c r="R156"/>
-    </row>
-    <row r="157" spans="1:18">
-      <c r="A157" s="1">
-        <v>44874.291666666664</v>
-      </c>
-      <c r="B157"/>
-      <c r="C157"/>
-      <c r="D157"/>
-      <c r="E157"/>
-      <c r="F157"/>
-      <c r="G157"/>
-      <c r="H157"/>
-      <c r="I157"/>
-      <c r="J157"/>
-      <c r="K157"/>
-      <c r="L157"/>
-      <c r="M157"/>
-      <c r="N157"/>
-      <c r="O157"/>
-      <c r="P157"/>
-      <c r="Q157"/>
-      <c r="R157"/>
-    </row>
-    <row r="158" spans="1:18">
-      <c r="A158" s="1">
-        <v>44874.302083333336</v>
-      </c>
-      <c r="B158"/>
-      <c r="C158"/>
-      <c r="D158"/>
-      <c r="E158"/>
-      <c r="F158"/>
-      <c r="G158"/>
-      <c r="H158"/>
-      <c r="I158"/>
-      <c r="J158"/>
-      <c r="K158"/>
-      <c r="L158"/>
-      <c r="M158"/>
-      <c r="N158"/>
-      <c r="O158"/>
-      <c r="P158"/>
-      <c r="Q158"/>
-      <c r="R158"/>
-    </row>
-    <row r="159" spans="1:18">
-      <c r="A159" s="1">
-        <v>44874.3125</v>
-      </c>
-      <c r="B159"/>
-      <c r="C159"/>
-      <c r="D159"/>
-      <c r="E159"/>
-      <c r="F159"/>
-      <c r="G159"/>
-      <c r="H159"/>
-      <c r="I159"/>
-      <c r="J159"/>
-      <c r="K159"/>
-      <c r="L159"/>
-      <c r="M159"/>
-      <c r="N159"/>
-      <c r="O159"/>
-      <c r="P159"/>
-      <c r="Q159"/>
-      <c r="R159"/>
-    </row>
-    <row r="160" spans="1:18">
-      <c r="A160" s="1">
-        <v>44874.322916666664</v>
-      </c>
-      <c r="B160"/>
-      <c r="C160"/>
-      <c r="D160"/>
-      <c r="E160"/>
-      <c r="F160"/>
-      <c r="G160"/>
-      <c r="H160"/>
-      <c r="I160"/>
-      <c r="J160"/>
-      <c r="K160"/>
-      <c r="L160"/>
-      <c r="M160"/>
-      <c r="N160"/>
-      <c r="O160"/>
-      <c r="P160"/>
-      <c r="Q160"/>
-      <c r="R160"/>
-    </row>
-    <row r="161" spans="1:18">
-      <c r="A161" s="1">
-        <v>44874.333333333336</v>
-      </c>
-      <c r="B161"/>
-      <c r="C161"/>
-      <c r="D161"/>
-      <c r="E161"/>
-      <c r="F161"/>
-      <c r="G161"/>
-      <c r="H161"/>
-      <c r="I161"/>
-      <c r="J161"/>
-      <c r="K161"/>
-      <c r="L161"/>
-      <c r="M161"/>
-      <c r="N161"/>
-      <c r="O161"/>
-      <c r="P161"/>
-      <c r="Q161"/>
-      <c r="R161"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>